<commit_message>
Ajout du script de Google Analytics
</commit_message>
<xml_diff>
--- a/rapport/Rapport SEO.xlsx
+++ b/rapport/Rapport SEO.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonic\Documents\formation_developpement\OpenClassrooms\projetoc_4\GregorhyAdrea_4_lapanthere_20221001\rapport\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49053477-9D96-4EDC-924D-1318F349E997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5460" yWindow="3585" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,63 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+  <si>
+    <t>TÂCHE OU TITRE</t>
+  </si>
+  <si>
+    <t>CRÉER UNE LISTE</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>ÉLÉMENT</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Élément</t>
+  </si>
+  <si>
+    <t>Remarque</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -37,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,18 +102,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Date" xfId="3" xr:uid="{8791FD49-078F-45C6-A09E-615CABB1C5A6}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <border>
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="4"/>
+      </font>
+      <border>
+        <horizontal style="medium">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Tâches" pivot="0" count="3" xr9:uid="{0AA09D83-102A-4763-A4F0-3538A708C4F1}">
+      <tableStyleElement type="wholeTable" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstColumn" dxfId="1"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -66,6 +226,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4CF10A6F-62C6-4EAF-BB34-04E3DE5D2D67}" name="Liste" displayName="Liste" ref="A3:C7">
+  <autoFilter ref="A3:C7" xr:uid="{4CF10A6F-62C6-4EAF-BB34-04E3DE5D2D67}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E0B4A522-BC2C-42FC-9B41-878F48E597C1}" name="DATE" totalsRowLabel="Total" totalsRowDxfId="0" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{04B58F77-8563-4F69-A3F4-194C6414BBCD}" name="ÉLÉMENT"/>
+    <tableColumn id="3" xr3:uid="{E80736AA-2C58-417C-8D25-B53AAAB9EF12}" name="NOTES" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="Tâches" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Entrez des dates, des éléments et des notes pour une créer une liste de tâches."/>
+    </ext>
+  </extLst>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +507,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez une tâche ou un titre dans cette cellule." sqref="A1" xr:uid="{58DE77EB-F832-43B0-9958-7F845278067F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Le titre de cette feuille de calcul figure dans cette cellule." sqref="A2" xr:uid="{14C32F61-2D17-4464-9107-7EC9EB860E77}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez la date dans cette colonne sous ce titre. Utilisez les filtres des titres pour trouver des entrées spécifiques" sqref="A3" xr:uid="{A8A1A714-13A5-4C2E-B70B-911783F4C383}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez la tâche dans cette colonne sous ce titre." sqref="B3" xr:uid="{3066A6DD-12A1-4AD1-ACA0-D94289C6614D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez les notes dans cette colonne sous ce titre." sqref="C3" xr:uid="{DCA79E43-2B90-4CA0-BAFF-A3DB6BF1EAE9}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modification des fichiers de rapport selon les directives du projet
</commit_message>
<xml_diff>
--- a/rapport/Rapport SEO.xlsx
+++ b/rapport/Rapport SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonic\Documents\formation_developpement\OpenClassrooms\projetoc_4\GregorhyAdrea_4_lapanthere_20221001\rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49053477-9D96-4EDC-924D-1318F349E997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CEF2C7-0665-4792-A7D7-7AAB8432E643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="3585" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2010" yWindow="4080" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,22 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
-  <si>
-    <t>TÂCHE OU TITRE</t>
-  </si>
-  <si>
-    <t>CRÉER UNE LISTE</t>
-  </si>
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>ÉLÉMENT</t>
-  </si>
-  <si>
-    <t>NOTES</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -49,13 +34,37 @@
   </si>
   <si>
     <t>Remarque</t>
+  </si>
+  <si>
+    <t>Analyse SEO / Performance</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>Problème identifié</t>
+  </si>
+  <si>
+    <t>Explication du problème</t>
+  </si>
+  <si>
+    <t>Bonne pratique à adopter</t>
+  </si>
+  <si>
+    <t>Action recommandée</t>
+  </si>
+  <si>
+    <t>Référence</t>
+  </si>
+  <si>
+    <t>Catégorie (SEO? Performance? Accessibilité?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,13 +94,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -120,7 +142,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -134,6 +156,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Date" xfId="3" xr:uid="{8791FD49-078F-45C6-A09E-615CABB1C5A6}"/>
@@ -141,7 +166,40 @@
     <cellStyle name="Titre" xfId="1" builtinId="15"/>
     <cellStyle name="Titre 1" xfId="2" builtinId="16"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -212,9 +270,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Tâches" pivot="0" count="3" xr9:uid="{0AA09D83-102A-4763-A4F0-3538A708C4F1}">
-      <tableStyleElement type="wholeTable" dxfId="3"/>
-      <tableStyleElement type="headerRow" dxfId="2"/>
-      <tableStyleElement type="firstColumn" dxfId="1"/>
+      <tableStyleElement type="wholeTable" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="firstColumn" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -232,9 +290,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4CF10A6F-62C6-4EAF-BB34-04E3DE5D2D67}" name="Liste" displayName="Liste" ref="A3:C7">
   <autoFilter ref="A3:C7" xr:uid="{4CF10A6F-62C6-4EAF-BB34-04E3DE5D2D67}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E0B4A522-BC2C-42FC-9B41-878F48E597C1}" name="DATE" totalsRowLabel="Total" totalsRowDxfId="0" dataCellStyle="Date"/>
-    <tableColumn id="2" xr3:uid="{04B58F77-8563-4F69-A3F4-194C6414BBCD}" name="ÉLÉMENT"/>
-    <tableColumn id="3" xr3:uid="{E80736AA-2C58-417C-8D25-B53AAAB9EF12}" name="NOTES" totalsRowFunction="count"/>
+    <tableColumn id="1" xr3:uid="{E0B4A522-BC2C-42FC-9B41-878F48E597C1}" name="Catégorie (SEO? Performance? Accessibilité?)" totalsRowLabel="Total" totalsRowDxfId="1" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{04B58F77-8563-4F69-A3F4-194C6414BBCD}" name="Problème identifié"/>
+    <tableColumn id="3" xr3:uid="{E80736AA-2C58-417C-8D25-B53AAAB9EF12}" name="Explication du problème" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="Tâches" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Entrez des dates, des éléments et des notes pour une créer une liste de tâches."/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90C1EE89-25D0-4F5F-833B-2909C664D289}" name="Liste3" displayName="Liste3" ref="D3:F7">
+  <autoFilter ref="D3:F7" xr:uid="{90C1EE89-25D0-4F5F-833B-2909C664D289}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{405B9B1A-9774-4147-B940-155318907196}" name="Bonne pratique à adopter" totalsRowLabel="Total" totalsRowDxfId="0" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{20A94986-C5A6-4178-AABA-04F7381C771C}" name="Action recommandée"/>
+    <tableColumn id="3" xr3:uid="{5C4DC0BC-AFA0-49C5-9366-3228F0E151D0}" name="Référence" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="Tâches" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -508,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,106 +594,143 @@
     <col min="1" max="1" width="36" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="6" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -633,13 +745,15 @@
   <dataValidations count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez une tâche ou un titre dans cette cellule." sqref="A1" xr:uid="{58DE77EB-F832-43B0-9958-7F845278067F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Le titre de cette feuille de calcul figure dans cette cellule." sqref="A2" xr:uid="{14C32F61-2D17-4464-9107-7EC9EB860E77}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez la date dans cette colonne sous ce titre. Utilisez les filtres des titres pour trouver des entrées spécifiques" sqref="A3" xr:uid="{A8A1A714-13A5-4C2E-B70B-911783F4C383}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez la tâche dans cette colonne sous ce titre." sqref="B3" xr:uid="{3066A6DD-12A1-4AD1-ACA0-D94289C6614D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez les notes dans cette colonne sous ce titre." sqref="C3" xr:uid="{DCA79E43-2B90-4CA0-BAFF-A3DB6BF1EAE9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez la date dans cette colonne sous ce titre. Utilisez les filtres des titres pour trouver des entrées spécifiques" sqref="A3 D3" xr:uid="{A8A1A714-13A5-4C2E-B70B-911783F4C383}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez la tâche dans cette colonne sous ce titre." sqref="B3 E3" xr:uid="{3066A6DD-12A1-4AD1-ACA0-D94289C6614D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez les notes dans cette colonne sous ce titre." sqref="C3 F3" xr:uid="{DCA79E43-2B90-4CA0-BAFF-A3DB6BF1EAE9}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>